<commit_message>
Cambios en la inversión de tiempo. Corte 2
</commit_message>
<xml_diff>
--- a/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
+++ b/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57BC87F-646B-4B12-B31D-A099D13F09CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E7E1F8-57A9-410E-8518-C8A33B7BF2D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>No.</t>
   </si>
@@ -68,6 +68,36 @@
   </si>
   <si>
     <t>Esta persona ha participado en distintas elecciones. Prefiere algunas cosas que se han hecho y otras que no.</t>
+  </si>
+  <si>
+    <t>Creación de Story Boards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizaron 2 story boards. </t>
+  </si>
+  <si>
+    <t>Design Thinking - Lluvia de Ideas</t>
+  </si>
+  <si>
+    <t>Avances 2 Corte</t>
+  </si>
+  <si>
+    <t>Design Thinking - Necesidades y Conclusión</t>
+  </si>
+  <si>
+    <t>Se realizó la lluvia de ideas entre personas del grupo y la votación</t>
+  </si>
+  <si>
+    <t>Se realizó las ideas más votadas y se dejaron claras para los story boards</t>
+  </si>
+  <si>
+    <t>Documento 2 Corte</t>
+  </si>
+  <si>
+    <t>2 Corte</t>
+  </si>
+  <si>
+    <t>creación de documento, llenado de inversión de tiempo y bitácora de grupo</t>
   </si>
 </sst>
 </file>
@@ -103,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -116,6 +146,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,19 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -530,28 +572,28 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>43506</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>9.375E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -559,32 +601,148 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>43506</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>10</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7">
+        <v>43528</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F8" s="4">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4">
+        <v>75</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7">
+        <v>43528</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F9" s="4">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4">
+        <v>75</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7">
+        <v>43529</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.1875</v>
+      </c>
+      <c r="F10" s="4">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4">
+        <v>120</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7">
+        <v>43538</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F11" s="4">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4">
+        <v>180</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en la inversion de tiempo TEjada Corte 2
</commit_message>
<xml_diff>
--- a/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
+++ b/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E7E1F8-57A9-410E-8518-C8A33B7BF2D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD33E5F-4EE2-4B9C-857D-BBBC99B2BF39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>No.</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>creación de documento, llenado de inversión de tiempo y bitácora de grupo</t>
+  </si>
+  <si>
+    <t>Se llamó a la persona ciega y se preguntó por dudas y otras cuestiones relacionadas con el proceso para personas con necesidades especiales</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I11"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,32 +719,61 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C11" s="7">
-        <v>43538</v>
+        <v>43531</v>
       </c>
       <c r="D11" s="8">
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E11" s="8">
         <v>0.47916666666666669</v>
       </c>
       <c r="F11" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G11" s="4">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="7">
+        <v>43538</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F12" s="4">
+        <v>30</v>
+      </c>
+      <c r="G12" s="4">
+        <v>180</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inversión de tiempo -corte 3
</commit_message>
<xml_diff>
--- a/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
+++ b/Inversiones de Tiempo/Inversión Tiempo - Alejandro Tejada.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD33E5F-4EE2-4B9C-857D-BBBC99B2BF39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F74DBDE-413E-46F0-A82E-57404401DE58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>No.</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Se llamó a la persona ciega y se preguntó por dudas y otras cuestiones relacionadas con el proceso para personas con necesidades especiales</t>
+  </si>
+  <si>
+    <t>3 Corte</t>
+  </si>
+  <si>
+    <t>Investigación de tecnología a utilizar</t>
+  </si>
+  <si>
+    <t>Se hizo la investigación sobre las tecnologías que se tendrían que usar para la entrega. En especiala, de .NET y React</t>
   </si>
 </sst>
 </file>
@@ -136,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,6 +171,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I12"/>
+  <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,6 +788,35 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="9">
+        <v>43550</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F13" s="4">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <v>170</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>